<commit_message>
Revisione checklist come richiesto
commonName auth: "A1#111EXPRIVIA000"
subject_application_vendor: "exprivia"
subject_application_id: "eris"
subject_application_version: "5"
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111EXPRIVIA000/EXPRIVIA/ERIS/5/report-checklist.xlsx
+++ b/GATEWAY/A1#111EXPRIVIA000/EXPRIVIA/ERIS/5/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://exprivia.sharepoint.com/sites/DFEH-PS-FSE2.0adeguamenti/Documenti condivisi/Documenti Accreditamento/Accreditamento ERIS/2023-04-06 - REVISIONE ACCREDITAMENTO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="251" documentId="8_{DC21B97C-41D4-4328-A083-28BBC17E4B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F2AD184-0D8D-4717-9C67-A684C253523C}"/>
+  <xr:revisionPtr revIDLastSave="287" documentId="8_{DC21B97C-41D4-4328-A083-28BBC17E4B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD5C5242-A040-44E5-8CA5-7EBAE538B055}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="240" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="5" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="369">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1550,9 +1550,6 @@
     <t>il Tag &lt;addr&gt; non è gestito perchè opzionale e per via dell'ereditarietà dell'opzionalità.</t>
   </si>
   <si>
-    <t>Segnalato tramite sistema di monitoraggio</t>
-  </si>
-  <si>
     <t>connection timeout</t>
   </si>
   <si>
@@ -1594,6 +1591,18 @@
   </si>
   <si>
     <t>"title":"Campo token JWT non valido.","detail":"Il codice fiscale nel campo sub non è corretto","status":403,"instance":"/jwt-mandatory-field-malformed"</t>
+  </si>
+  <si>
+    <t>In caso di errore viene mostrato l'errore all'utente.
+E' possibile configurare se interrompere o portare a termine il processo di firma.
+L'errore viene tracciato nei relativi log.
+In backoffice si potrà correggere e procedere al reinvio o alla richiesta al medico di creare una nuova versione del referto.</t>
+  </si>
+  <si>
+    <t>E' possibile configurare i ms di timeout ed il numero di tentativi da effettuare prima di restituire l'errore di timeout all'utente.
+In questo caso viene mostrato l'errore all'utente.
+L'errore viene tracciato nei relativi log.
+In backoffice si potrà procedere al reinvio.</t>
   </si>
 </sst>
 </file>
@@ -2100,7 +2109,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -2244,6 +2253,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -2283,6 +2295,10 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -3732,11 +3748,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T992"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3756,7 +3772,7 @@
     <col min="13" max="13" width="24.85546875" style="22" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="25.5703125" style="22" customWidth="1"/>
     <col min="15" max="15" width="29.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="58" style="22" customWidth="1"/>
     <col min="17" max="17" width="11.5703125" style="22" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="31.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11.42578125" style="22" bestFit="1" customWidth="1"/>
@@ -3782,14 +3798,14 @@
       <c r="T1" s="24"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53" t="s">
+      <c r="B2" s="53"/>
+      <c r="C2" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="52"/>
+      <c r="D2" s="53"/>
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
@@ -3807,14 +3823,14 @@
       <c r="T2" s="24"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="60" t="s">
+      <c r="B3" s="56"/>
+      <c r="C3" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="52"/>
+      <c r="D3" s="53"/>
       <c r="F3" s="23"/>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
@@ -3832,12 +3848,12 @@
       <c r="T3" s="24"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="56"/>
-      <c r="B4" s="57"/>
-      <c r="C4" s="60" t="s">
+      <c r="A4" s="57"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="52"/>
+      <c r="D4" s="53"/>
       <c r="E4" s="26"/>
       <c r="F4" s="23"/>
       <c r="G4" s="23"/>
@@ -3856,12 +3872,12 @@
       <c r="T4" s="24"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="58"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="60" t="s">
+      <c r="A5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="52"/>
+      <c r="D5" s="53"/>
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
@@ -3879,8 +3895,8 @@
       <c r="T5" s="24"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="49"/>
-      <c r="B6" s="50"/>
+      <c r="A6" s="50"/>
+      <c r="B6" s="51"/>
       <c r="C6" s="27"/>
       <c r="F6" s="23"/>
       <c r="G6" s="23"/>
@@ -4304,7 +4320,7 @@
       </c>
     </row>
     <row r="19" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="31">
+      <c r="A19" s="62">
         <v>11</v>
       </c>
       <c r="B19" s="32" t="s">
@@ -4323,13 +4339,13 @@
         <v>45022</v>
       </c>
       <c r="G19" s="35" t="s">
+        <v>356</v>
+      </c>
+      <c r="H19" s="35" t="s">
         <v>357</v>
       </c>
-      <c r="H19" s="35" t="s">
+      <c r="I19" s="35" t="s">
         <v>358</v>
-      </c>
-      <c r="I19" s="35" t="s">
-        <v>359</v>
       </c>
       <c r="J19" s="36" t="s">
         <v>69</v>
@@ -4367,13 +4383,13 @@
         <v>45022</v>
       </c>
       <c r="G20" s="35" t="s">
+        <v>359</v>
+      </c>
+      <c r="H20" s="35" t="s">
         <v>360</v>
       </c>
-      <c r="H20" s="35" t="s">
+      <c r="I20" s="35" t="s">
         <v>361</v>
-      </c>
-      <c r="I20" s="35" t="s">
-        <v>362</v>
       </c>
       <c r="J20" s="36" t="s">
         <v>69</v>
@@ -4415,7 +4431,7 @@
         <v>74</v>
       </c>
       <c r="K21" s="36" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="L21" s="36"/>
       <c r="M21" s="36"/>
@@ -4967,7 +4983,7 @@
         <v>74</v>
       </c>
       <c r="K37" s="36" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="L37" s="36"/>
       <c r="M37" s="36"/>
@@ -5171,10 +5187,10 @@
         <v>45022</v>
       </c>
       <c r="G43" s="35" t="s">
+        <v>364</v>
+      </c>
+      <c r="H43" s="35" t="s">
         <v>365</v>
-      </c>
-      <c r="H43" s="35" t="s">
-        <v>366</v>
       </c>
       <c r="I43" s="35" t="s">
         <v>111</v>
@@ -5190,16 +5206,16 @@
         <v>74</v>
       </c>
       <c r="N43" s="36" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="O43" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="P43" s="36" t="s">
-        <v>354</v>
+      <c r="P43" s="33" t="s">
+        <v>367</v>
       </c>
       <c r="Q43" s="36"/>
-      <c r="R43" s="39"/>
+      <c r="R43" s="49"/>
       <c r="S43" s="37"/>
       <c r="T43" s="40" t="s">
         <v>107</v>
@@ -5379,7 +5395,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="31">
         <v>47</v>
       </c>
@@ -5412,13 +5428,13 @@
         <v>74</v>
       </c>
       <c r="N49" s="36" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="O49" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="P49" s="36" t="s">
-        <v>354</v>
+      <c r="P49" s="33" t="s">
+        <v>368</v>
       </c>
       <c r="Q49" s="36"/>
       <c r="R49" s="39"/>
@@ -6622,13 +6638,13 @@
         <v>74</v>
       </c>
       <c r="N83" s="36" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="O83" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="P83" s="36" t="s">
-        <v>354</v>
+      <c r="P83" s="33" t="s">
+        <v>367</v>
       </c>
       <c r="Q83" s="36"/>
       <c r="R83" s="39"/>
@@ -8177,7 +8193,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="31">
         <v>127</v>
       </c>
@@ -8211,7 +8227,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="129" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="31">
         <v>128</v>
       </c>
@@ -8245,7 +8261,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="130" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="31">
         <v>129</v>
       </c>
@@ -8279,7 +8295,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="131" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="31">
         <v>130</v>
       </c>
@@ -8313,7 +8329,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="132" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="31">
         <v>131</v>
       </c>
@@ -8347,7 +8363,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="133" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="31">
         <v>132</v>
       </c>
@@ -8381,7 +8397,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="134" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="31">
         <v>133</v>
       </c>
@@ -8415,7 +8431,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="135" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="31">
         <v>134</v>
       </c>
@@ -8449,7 +8465,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="136" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="31">
         <v>135</v>
       </c>
@@ -8483,7 +8499,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="137" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="31">
         <v>136</v>
       </c>
@@ -8517,7 +8533,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="138" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="31">
         <v>137</v>
       </c>
@@ -8551,7 +8567,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="139" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="31">
         <v>138</v>
       </c>
@@ -8585,7 +8601,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="140" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="31">
         <v>139</v>
       </c>
@@ -8619,7 +8635,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="141" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="31">
         <v>140</v>
       </c>
@@ -8653,7 +8669,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="142" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="31">
         <v>141</v>
       </c>
@@ -8687,7 +8703,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="143" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="31">
         <v>142</v>
       </c>
@@ -8721,7 +8737,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="144" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="31">
         <v>143</v>
       </c>
@@ -8755,7 +8771,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="145" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="31">
         <v>144</v>
       </c>
@@ -8789,7 +8805,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="146" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="31">
         <v>145</v>
       </c>
@@ -8823,7 +8839,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="147" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="31">
         <v>146</v>
       </c>
@@ -25430,17 +25446,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100794258E7DE47134588D45098EBDB60F8" ma:contentTypeVersion="4" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="2dbc010f7356a33b20da83a73eb190a5">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0bdf65ce-24cf-486b-995b-57ece8b70f4e" xmlns:ns3="c50f76eb-a136-4a5c-b9b3-fbcc59ed104d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bbb2aea3e03736235287e3873b29b8db" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100794258E7DE47134588D45098EBDB60F8" ma:contentTypeVersion="6" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="3194f2ccada4dbd4f766fc5cce730de0">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0bdf65ce-24cf-486b-995b-57ece8b70f4e" xmlns:ns3="c50f76eb-a136-4a5c-b9b3-fbcc59ed104d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0b17b18953fe681e8c031b46ce8399c7" ns2:_="" ns3:_="">
     <xsd:import namespace="0bdf65ce-24cf-486b-995b-57ece8b70f4e"/>
     <xsd:import namespace="c50f76eb-a136-4a5c-b9b3-fbcc59ed104d"/>
     <xsd:element name="properties">
@@ -25453,6 +25466,8 @@
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -25471,6 +25486,16 @@
     <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="12" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="13" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -25604,21 +25629,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B29C747-7E08-4ADD-838E-37132E454A5C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D366502-F098-4D33-AC4B-3B90E4A01E18}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -25637,10 +25666,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Revisione checklist gestione errore
commonName auth: "A1#111EXPRIVIA000"
subject_application_vendor: "exprivia"
subject_application_id: "eris"
subject_application_version: "5"
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111EXPRIVIA000/EXPRIVIA/ERIS/5/report-checklist.xlsx
+++ b/GATEWAY/A1#111EXPRIVIA000/EXPRIVIA/ERIS/5/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://exprivia.sharepoint.com/sites/DFEH-PS-FSE2.0adeguamenti/Documenti condivisi/Documenti Accreditamento/Accreditamento ERIS/2023-04-06 - REVISIONE ACCREDITAMENTO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="287" documentId="8_{DC21B97C-41D4-4328-A083-28BBC17E4B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD5C5242-A040-44E5-8CA5-7EBAE538B055}"/>
+  <xr:revisionPtr revIDLastSave="294" documentId="8_{DC21B97C-41D4-4328-A083-28BBC17E4B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1062AD2B-0953-4ADA-AA44-6C3E16353CCA}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2256,6 +2256,10 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -2295,10 +2299,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -3749,10 +3749,10 @@
   <dimension ref="A1:T992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F93" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomRight" activeCell="M49" sqref="M49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3798,14 +3798,14 @@
       <c r="T1" s="24"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="54" t="s">
+      <c r="B2" s="54"/>
+      <c r="C2" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="53"/>
+      <c r="D2" s="54"/>
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
@@ -3823,14 +3823,14 @@
       <c r="T2" s="24"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="61" t="s">
+      <c r="B3" s="57"/>
+      <c r="C3" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="53"/>
+      <c r="D3" s="54"/>
       <c r="F3" s="23"/>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
@@ -3848,12 +3848,12 @@
       <c r="T3" s="24"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="57"/>
-      <c r="B4" s="58"/>
-      <c r="C4" s="61" t="s">
+      <c r="A4" s="58"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="53"/>
+      <c r="D4" s="54"/>
       <c r="E4" s="26"/>
       <c r="F4" s="23"/>
       <c r="G4" s="23"/>
@@ -3872,12 +3872,12 @@
       <c r="T4" s="24"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="59"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="61" t="s">
+      <c r="A5" s="60"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="53"/>
+      <c r="D5" s="54"/>
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
@@ -3895,8 +3895,8 @@
       <c r="T5" s="24"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="50"/>
-      <c r="B6" s="51"/>
+      <c r="A6" s="51"/>
+      <c r="B6" s="52"/>
       <c r="C6" s="27"/>
       <c r="F6" s="23"/>
       <c r="G6" s="23"/>
@@ -4320,7 +4320,7 @@
       </c>
     </row>
     <row r="19" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="62">
+      <c r="A19" s="50">
         <v>11</v>
       </c>
       <c r="B19" s="32" t="s">
@@ -5203,7 +5203,7 @@
         <v>69</v>
       </c>
       <c r="M43" s="36" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="N43" s="36" t="s">
         <v>366</v>
@@ -5425,7 +5425,7 @@
         <v>74</v>
       </c>
       <c r="M49" s="36" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="N49" s="36" t="s">
         <v>354</v>
@@ -6635,7 +6635,7 @@
         <v>74</v>
       </c>
       <c r="M83" s="36" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="N83" s="36" t="s">
         <v>355</v>
@@ -8193,7 +8193,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="31">
         <v>127</v>
       </c>
@@ -8227,7 +8227,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="129" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="31">
         <v>128</v>
       </c>
@@ -8261,7 +8261,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="130" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="31">
         <v>129</v>
       </c>
@@ -8295,7 +8295,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="131" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="31">
         <v>130</v>
       </c>
@@ -8329,7 +8329,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="132" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="31">
         <v>131</v>
       </c>
@@ -8363,7 +8363,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="133" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="31">
         <v>132</v>
       </c>
@@ -8397,7 +8397,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="134" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="31">
         <v>133</v>
       </c>
@@ -8431,7 +8431,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="135" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="31">
         <v>134</v>
       </c>
@@ -8465,7 +8465,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="136" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="31">
         <v>135</v>
       </c>
@@ -8499,7 +8499,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="137" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="31">
         <v>136</v>
       </c>
@@ -8533,7 +8533,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="138" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="31">
         <v>137</v>
       </c>
@@ -8567,7 +8567,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="139" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="31">
         <v>138</v>
       </c>
@@ -8601,7 +8601,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="140" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="31">
         <v>139</v>
       </c>
@@ -8635,7 +8635,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="141" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="31">
         <v>140</v>
       </c>
@@ -8669,7 +8669,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="142" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="31">
         <v>141</v>
       </c>
@@ -8703,7 +8703,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="143" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="31">
         <v>142</v>
       </c>
@@ -8737,7 +8737,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="144" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="31">
         <v>143</v>
       </c>
@@ -8771,7 +8771,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="145" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="31">
         <v>144</v>
       </c>
@@ -8805,7 +8805,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="146" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="31">
         <v>145</v>
       </c>
@@ -8839,7 +8839,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="147" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="31">
         <v>146</v>
       </c>

</xml_diff>

<commit_message>
Revisione Checklist CT5 id75
commonName auth: "A1#111EXPRIVIA000"
subject_application_vendor: "exprivia"
subject_application_id: "eris"
subject_application_version: "5"
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111EXPRIVIA000/EXPRIVIA/ERIS/5/report-checklist.xlsx
+++ b/GATEWAY/A1#111EXPRIVIA000/EXPRIVIA/ERIS/5/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://exprivia.sharepoint.com/sites/DFEH-PS-FSE2.0adeguamenti/Documenti condivisi/Documenti Accreditamento/Accreditamento ERIS/2023-04-06 - REVISIONE ACCREDITAMENTO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="294" documentId="8_{DC21B97C-41D4-4328-A083-28BBC17E4B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1062AD2B-0953-4ADA-AA44-6C3E16353CCA}"/>
+  <xr:revisionPtr revIDLastSave="298" documentId="8_{DC21B97C-41D4-4328-A083-28BBC17E4B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E5E8C80-0C79-4B24-A13B-4ECF5CA7FC7F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -905,9 +905,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>IdPaziente campo obbligatorio su applicativo</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_RAD_CT6_KO</t>
   </si>
   <si>
@@ -1581,9 +1578,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">I parametri del token JWT possono essere valorizzati in maniera errata ma non possono essere mancanti. </t>
-  </si>
-  <si>
     <t>2023-04-06T12:27:32Z</t>
   </si>
   <si>
@@ -1603,6 +1597,12 @@
 In questo caso viene mostrato l'errore all'utente.
 L'errore viene tracciato nei relativi log.
 In backoffice si potrà procedere al reinvio.</t>
+  </si>
+  <si>
+    <t>confidentialityCode campo obbligatorio su applicativo</t>
+  </si>
+  <si>
+    <t>I parametri del token JWT possono essere valorizzati in maniera errata ma non possono essere mancanti.</t>
   </si>
 </sst>
 </file>
@@ -3749,10 +3749,10 @@
   <dimension ref="A1:T992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F93" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="M49" sqref="M49"/>
+      <selection pane="bottomRight" activeCell="K76" sqref="K76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4319,7 +4319,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="50">
         <v>11</v>
       </c>
@@ -4339,13 +4339,13 @@
         <v>45022</v>
       </c>
       <c r="G19" s="35" t="s">
+        <v>355</v>
+      </c>
+      <c r="H19" s="35" t="s">
         <v>356</v>
       </c>
-      <c r="H19" s="35" t="s">
+      <c r="I19" s="35" t="s">
         <v>357</v>
-      </c>
-      <c r="I19" s="35" t="s">
-        <v>358</v>
       </c>
       <c r="J19" s="36" t="s">
         <v>69</v>
@@ -4363,7 +4363,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="31">
         <v>12</v>
       </c>
@@ -4383,13 +4383,13 @@
         <v>45022</v>
       </c>
       <c r="G20" s="35" t="s">
+        <v>358</v>
+      </c>
+      <c r="H20" s="35" t="s">
         <v>359</v>
       </c>
-      <c r="H20" s="35" t="s">
+      <c r="I20" s="35" t="s">
         <v>360</v>
-      </c>
-      <c r="I20" s="35" t="s">
-        <v>361</v>
       </c>
       <c r="J20" s="36" t="s">
         <v>69</v>
@@ -4431,7 +4431,7 @@
         <v>74</v>
       </c>
       <c r="K21" s="36" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="L21" s="36"/>
       <c r="M21" s="36"/>
@@ -4983,7 +4983,7 @@
         <v>74</v>
       </c>
       <c r="K37" s="36" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="L37" s="36"/>
       <c r="M37" s="36"/>
@@ -5167,7 +5167,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="31">
         <v>39</v>
       </c>
@@ -5187,10 +5187,10 @@
         <v>45022</v>
       </c>
       <c r="G43" s="35" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="H43" s="35" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="I43" s="35" t="s">
         <v>111</v>
@@ -5206,13 +5206,13 @@
         <v>69</v>
       </c>
       <c r="N43" s="36" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="O43" s="36" t="s">
         <v>69</v>
       </c>
       <c r="P43" s="33" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="Q43" s="36"/>
       <c r="R43" s="49"/>
@@ -5395,7 +5395,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="31">
         <v>47</v>
       </c>
@@ -5428,13 +5428,13 @@
         <v>69</v>
       </c>
       <c r="N49" s="36" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="O49" s="36" t="s">
         <v>69</v>
       </c>
       <c r="P49" s="33" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="Q49" s="36"/>
       <c r="R49" s="39"/>
@@ -6357,7 +6357,7 @@
         <v>74</v>
       </c>
       <c r="K76" s="36" t="s">
-        <v>177</v>
+        <v>367</v>
       </c>
       <c r="L76" s="36"/>
       <c r="M76" s="36"/>
@@ -6382,10 +6382,10 @@
         <v>66</v>
       </c>
       <c r="D77" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="E77" s="33" t="s">
         <v>178</v>
-      </c>
-      <c r="E77" s="33" t="s">
-        <v>179</v>
       </c>
       <c r="F77" s="34"/>
       <c r="G77" s="35"/>
@@ -6395,7 +6395,7 @@
         <v>74</v>
       </c>
       <c r="K77" s="36" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L77" s="36"/>
       <c r="M77" s="36"/>
@@ -6420,10 +6420,10 @@
         <v>66</v>
       </c>
       <c r="D78" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="E78" s="33" t="s">
         <v>181</v>
-      </c>
-      <c r="E78" s="33" t="s">
-        <v>182</v>
       </c>
       <c r="F78" s="34"/>
       <c r="G78" s="35"/>
@@ -6433,7 +6433,7 @@
         <v>74</v>
       </c>
       <c r="K78" s="36" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L78" s="36"/>
       <c r="M78" s="36"/>
@@ -6458,10 +6458,10 @@
         <v>66</v>
       </c>
       <c r="D79" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="E79" s="33" t="s">
         <v>184</v>
-      </c>
-      <c r="E79" s="33" t="s">
-        <v>185</v>
       </c>
       <c r="F79" s="34"/>
       <c r="G79" s="35"/>
@@ -6471,7 +6471,7 @@
         <v>74</v>
       </c>
       <c r="K79" s="36" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="L79" s="36"/>
       <c r="M79" s="36"/>
@@ -6496,10 +6496,10 @@
         <v>66</v>
       </c>
       <c r="D80" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="E80" s="33" t="s">
         <v>186</v>
-      </c>
-      <c r="E80" s="33" t="s">
-        <v>187</v>
       </c>
       <c r="F80" s="34"/>
       <c r="G80" s="35"/>
@@ -6509,7 +6509,7 @@
         <v>74</v>
       </c>
       <c r="K80" s="36" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L80" s="36"/>
       <c r="M80" s="36"/>
@@ -6534,10 +6534,10 @@
         <v>66</v>
       </c>
       <c r="D81" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="E81" s="33" t="s">
         <v>189</v>
-      </c>
-      <c r="E81" s="33" t="s">
-        <v>190</v>
       </c>
       <c r="F81" s="34"/>
       <c r="G81" s="35"/>
@@ -6547,7 +6547,7 @@
         <v>74</v>
       </c>
       <c r="K81" s="36" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="L81" s="36"/>
       <c r="M81" s="36"/>
@@ -6572,10 +6572,10 @@
         <v>66</v>
       </c>
       <c r="D82" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="E82" s="33" t="s">
         <v>192</v>
-      </c>
-      <c r="E82" s="33" t="s">
-        <v>193</v>
       </c>
       <c r="F82" s="34"/>
       <c r="G82" s="35"/>
@@ -6585,7 +6585,7 @@
         <v>74</v>
       </c>
       <c r="K82" s="36" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L82" s="36"/>
       <c r="M82" s="36"/>
@@ -6599,7 +6599,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="345.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:20" ht="345.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="31">
         <v>82</v>
       </c>
@@ -6610,22 +6610,22 @@
         <v>66</v>
       </c>
       <c r="D83" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="E83" s="33" t="s">
         <v>195</v>
-      </c>
-      <c r="E83" s="33" t="s">
-        <v>196</v>
       </c>
       <c r="F83" s="34">
         <v>45000</v>
       </c>
       <c r="G83" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="H83" s="43" t="s">
         <v>197</v>
       </c>
-      <c r="H83" s="43" t="s">
+      <c r="I83" s="35" t="s">
         <v>198</v>
-      </c>
-      <c r="I83" s="35" t="s">
-        <v>199</v>
       </c>
       <c r="J83" s="36" t="s">
         <v>69</v>
@@ -6638,13 +6638,13 @@
         <v>69</v>
       </c>
       <c r="N83" s="36" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="O83" s="36" t="s">
         <v>69</v>
       </c>
       <c r="P83" s="33" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="Q83" s="36"/>
       <c r="R83" s="39"/>
@@ -6664,10 +6664,10 @@
         <v>66</v>
       </c>
       <c r="D84" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="E84" s="33" t="s">
         <v>200</v>
-      </c>
-      <c r="E84" s="33" t="s">
-        <v>201</v>
       </c>
       <c r="F84" s="34"/>
       <c r="G84" s="35"/>
@@ -6677,7 +6677,7 @@
         <v>74</v>
       </c>
       <c r="K84" s="36" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L84" s="36"/>
       <c r="M84" s="36"/>
@@ -6702,10 +6702,10 @@
         <v>66</v>
       </c>
       <c r="D85" s="32" t="s">
+        <v>202</v>
+      </c>
+      <c r="E85" s="33" t="s">
         <v>203</v>
-      </c>
-      <c r="E85" s="33" t="s">
-        <v>204</v>
       </c>
       <c r="F85" s="34"/>
       <c r="G85" s="35"/>
@@ -6715,7 +6715,7 @@
         <v>74</v>
       </c>
       <c r="K85" s="36" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L85" s="36"/>
       <c r="M85" s="36"/>
@@ -6740,10 +6740,10 @@
         <v>66</v>
       </c>
       <c r="D86" s="32" t="s">
+        <v>205</v>
+      </c>
+      <c r="E86" s="33" t="s">
         <v>206</v>
-      </c>
-      <c r="E86" s="33" t="s">
-        <v>207</v>
       </c>
       <c r="F86" s="34"/>
       <c r="G86" s="35"/>
@@ -6753,7 +6753,7 @@
         <v>74</v>
       </c>
       <c r="K86" s="36" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L86" s="36"/>
       <c r="M86" s="36"/>
@@ -6778,10 +6778,10 @@
         <v>66</v>
       </c>
       <c r="D87" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="E87" s="33" t="s">
         <v>209</v>
-      </c>
-      <c r="E87" s="33" t="s">
-        <v>210</v>
       </c>
       <c r="F87" s="34"/>
       <c r="G87" s="35"/>
@@ -6791,7 +6791,7 @@
         <v>74</v>
       </c>
       <c r="K87" s="36" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L87" s="36"/>
       <c r="M87" s="36"/>
@@ -6816,10 +6816,10 @@
         <v>66</v>
       </c>
       <c r="D88" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="E88" s="33" t="s">
         <v>212</v>
-      </c>
-      <c r="E88" s="33" t="s">
-        <v>213</v>
       </c>
       <c r="F88" s="34"/>
       <c r="G88" s="35"/>
@@ -6829,7 +6829,7 @@
         <v>74</v>
       </c>
       <c r="K88" s="36" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="L88" s="36"/>
       <c r="M88" s="36"/>
@@ -6854,10 +6854,10 @@
         <v>66</v>
       </c>
       <c r="D89" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="E89" s="33" t="s">
         <v>215</v>
-      </c>
-      <c r="E89" s="33" t="s">
-        <v>216</v>
       </c>
       <c r="F89" s="34"/>
       <c r="G89" s="35"/>
@@ -6867,7 +6867,7 @@
         <v>74</v>
       </c>
       <c r="K89" s="36" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L89" s="36"/>
       <c r="M89" s="36"/>
@@ -6892,10 +6892,10 @@
         <v>66</v>
       </c>
       <c r="D90" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="E90" s="33" t="s">
         <v>218</v>
-      </c>
-      <c r="E90" s="33" t="s">
-        <v>219</v>
       </c>
       <c r="F90" s="34"/>
       <c r="G90" s="35"/>
@@ -6905,7 +6905,7 @@
         <v>74</v>
       </c>
       <c r="K90" s="36" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L90" s="36"/>
       <c r="M90" s="36"/>
@@ -6930,10 +6930,10 @@
         <v>66</v>
       </c>
       <c r="D91" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="E91" s="33" t="s">
         <v>220</v>
-      </c>
-      <c r="E91" s="33" t="s">
-        <v>221</v>
       </c>
       <c r="F91" s="34"/>
       <c r="G91" s="35"/>
@@ -6943,7 +6943,7 @@
         <v>74</v>
       </c>
       <c r="K91" s="36" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L91" s="36"/>
       <c r="M91" s="36"/>
@@ -6968,10 +6968,10 @@
         <v>66</v>
       </c>
       <c r="D92" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="E92" s="33" t="s">
         <v>222</v>
-      </c>
-      <c r="E92" s="33" t="s">
-        <v>223</v>
       </c>
       <c r="F92" s="34"/>
       <c r="G92" s="35"/>
@@ -6981,7 +6981,7 @@
         <v>74</v>
       </c>
       <c r="K92" s="36" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L92" s="36"/>
       <c r="M92" s="36"/>
@@ -7006,10 +7006,10 @@
         <v>66</v>
       </c>
       <c r="D93" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="E93" s="33" t="s">
         <v>224</v>
-      </c>
-      <c r="E93" s="33" t="s">
-        <v>225</v>
       </c>
       <c r="F93" s="34"/>
       <c r="G93" s="35"/>
@@ -7019,7 +7019,7 @@
         <v>74</v>
       </c>
       <c r="K93" s="36" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L93" s="36"/>
       <c r="M93" s="36"/>
@@ -7044,10 +7044,10 @@
         <v>66</v>
       </c>
       <c r="D94" s="32" t="s">
+        <v>226</v>
+      </c>
+      <c r="E94" s="33" t="s">
         <v>227</v>
-      </c>
-      <c r="E94" s="33" t="s">
-        <v>228</v>
       </c>
       <c r="F94" s="34"/>
       <c r="G94" s="35"/>
@@ -7057,7 +7057,7 @@
         <v>74</v>
       </c>
       <c r="K94" s="36" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L94" s="36"/>
       <c r="M94" s="36"/>
@@ -7082,10 +7082,10 @@
         <v>78</v>
       </c>
       <c r="D95" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="E95" s="33" t="s">
         <v>230</v>
-      </c>
-      <c r="E95" s="33" t="s">
-        <v>231</v>
       </c>
       <c r="F95" s="34"/>
       <c r="G95" s="35"/>
@@ -7116,10 +7116,10 @@
         <v>78</v>
       </c>
       <c r="D96" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="E96" s="33" t="s">
         <v>232</v>
-      </c>
-      <c r="E96" s="33" t="s">
-        <v>233</v>
       </c>
       <c r="F96" s="34"/>
       <c r="G96" s="35"/>
@@ -7150,10 +7150,10 @@
         <v>78</v>
       </c>
       <c r="D97" s="32" t="s">
+        <v>233</v>
+      </c>
+      <c r="E97" s="33" t="s">
         <v>234</v>
-      </c>
-      <c r="E97" s="33" t="s">
-        <v>235</v>
       </c>
       <c r="F97" s="34"/>
       <c r="G97" s="35"/>
@@ -7184,10 +7184,10 @@
         <v>78</v>
       </c>
       <c r="D98" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="E98" s="33" t="s">
         <v>236</v>
-      </c>
-      <c r="E98" s="33" t="s">
-        <v>237</v>
       </c>
       <c r="F98" s="34"/>
       <c r="G98" s="35"/>
@@ -7218,10 +7218,10 @@
         <v>78</v>
       </c>
       <c r="D99" s="32" t="s">
+        <v>237</v>
+      </c>
+      <c r="E99" s="33" t="s">
         <v>238</v>
-      </c>
-      <c r="E99" s="33" t="s">
-        <v>239</v>
       </c>
       <c r="F99" s="34"/>
       <c r="G99" s="35"/>
@@ -7252,10 +7252,10 @@
         <v>78</v>
       </c>
       <c r="D100" s="32" t="s">
+        <v>239</v>
+      </c>
+      <c r="E100" s="33" t="s">
         <v>240</v>
-      </c>
-      <c r="E100" s="33" t="s">
-        <v>241</v>
       </c>
       <c r="F100" s="34"/>
       <c r="G100" s="35"/>
@@ -7286,10 +7286,10 @@
         <v>78</v>
       </c>
       <c r="D101" s="32" t="s">
+        <v>241</v>
+      </c>
+      <c r="E101" s="33" t="s">
         <v>242</v>
-      </c>
-      <c r="E101" s="33" t="s">
-        <v>243</v>
       </c>
       <c r="F101" s="34"/>
       <c r="G101" s="35"/>
@@ -7320,10 +7320,10 @@
         <v>78</v>
       </c>
       <c r="D102" s="32" t="s">
+        <v>243</v>
+      </c>
+      <c r="E102" s="33" t="s">
         <v>244</v>
-      </c>
-      <c r="E102" s="33" t="s">
-        <v>245</v>
       </c>
       <c r="F102" s="34"/>
       <c r="G102" s="35"/>
@@ -7354,10 +7354,10 @@
         <v>78</v>
       </c>
       <c r="D103" s="32" t="s">
+        <v>245</v>
+      </c>
+      <c r="E103" s="33" t="s">
         <v>246</v>
-      </c>
-      <c r="E103" s="33" t="s">
-        <v>247</v>
       </c>
       <c r="F103" s="34"/>
       <c r="G103" s="35"/>
@@ -7388,10 +7388,10 @@
         <v>78</v>
       </c>
       <c r="D104" s="32" t="s">
+        <v>247</v>
+      </c>
+      <c r="E104" s="33" t="s">
         <v>248</v>
-      </c>
-      <c r="E104" s="33" t="s">
-        <v>249</v>
       </c>
       <c r="F104" s="34"/>
       <c r="G104" s="35"/>
@@ -7422,10 +7422,10 @@
         <v>78</v>
       </c>
       <c r="D105" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="E105" s="33" t="s">
         <v>250</v>
-      </c>
-      <c r="E105" s="33" t="s">
-        <v>251</v>
       </c>
       <c r="F105" s="34"/>
       <c r="G105" s="35"/>
@@ -7456,10 +7456,10 @@
         <v>78</v>
       </c>
       <c r="D106" s="32" t="s">
+        <v>251</v>
+      </c>
+      <c r="E106" s="33" t="s">
         <v>252</v>
-      </c>
-      <c r="E106" s="33" t="s">
-        <v>253</v>
       </c>
       <c r="F106" s="34"/>
       <c r="G106" s="35"/>
@@ -7490,10 +7490,10 @@
         <v>78</v>
       </c>
       <c r="D107" s="32" t="s">
+        <v>253</v>
+      </c>
+      <c r="E107" s="33" t="s">
         <v>254</v>
-      </c>
-      <c r="E107" s="33" t="s">
-        <v>255</v>
       </c>
       <c r="F107" s="34"/>
       <c r="G107" s="35"/>
@@ -7524,10 +7524,10 @@
         <v>87</v>
       </c>
       <c r="D108" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="E108" s="33" t="s">
         <v>256</v>
-      </c>
-      <c r="E108" s="33" t="s">
-        <v>257</v>
       </c>
       <c r="F108" s="34"/>
       <c r="G108" s="35"/>
@@ -7558,10 +7558,10 @@
         <v>87</v>
       </c>
       <c r="D109" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="E109" s="33" t="s">
         <v>258</v>
-      </c>
-      <c r="E109" s="33" t="s">
-        <v>259</v>
       </c>
       <c r="F109" s="34"/>
       <c r="G109" s="35"/>
@@ -7592,10 +7592,10 @@
         <v>87</v>
       </c>
       <c r="D110" s="32" t="s">
+        <v>259</v>
+      </c>
+      <c r="E110" s="33" t="s">
         <v>260</v>
-      </c>
-      <c r="E110" s="33" t="s">
-        <v>261</v>
       </c>
       <c r="F110" s="34"/>
       <c r="G110" s="35"/>
@@ -7626,10 +7626,10 @@
         <v>87</v>
       </c>
       <c r="D111" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="E111" s="33" t="s">
         <v>262</v>
-      </c>
-      <c r="E111" s="33" t="s">
-        <v>263</v>
       </c>
       <c r="F111" s="34"/>
       <c r="G111" s="35"/>
@@ -7660,10 +7660,10 @@
         <v>87</v>
       </c>
       <c r="D112" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="E112" s="33" t="s">
         <v>264</v>
-      </c>
-      <c r="E112" s="33" t="s">
-        <v>265</v>
       </c>
       <c r="F112" s="34"/>
       <c r="G112" s="35"/>
@@ -7694,10 +7694,10 @@
         <v>87</v>
       </c>
       <c r="D113" s="32" t="s">
+        <v>265</v>
+      </c>
+      <c r="E113" s="33" t="s">
         <v>266</v>
-      </c>
-      <c r="E113" s="33" t="s">
-        <v>267</v>
       </c>
       <c r="F113" s="34"/>
       <c r="G113" s="35"/>
@@ -7728,10 +7728,10 @@
         <v>87</v>
       </c>
       <c r="D114" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="E114" s="33" t="s">
         <v>268</v>
-      </c>
-      <c r="E114" s="33" t="s">
-        <v>269</v>
       </c>
       <c r="F114" s="34"/>
       <c r="G114" s="35"/>
@@ -7762,10 +7762,10 @@
         <v>87</v>
       </c>
       <c r="D115" s="32" t="s">
+        <v>269</v>
+      </c>
+      <c r="E115" s="33" t="s">
         <v>270</v>
-      </c>
-      <c r="E115" s="33" t="s">
-        <v>271</v>
       </c>
       <c r="F115" s="34"/>
       <c r="G115" s="35"/>
@@ -7796,10 +7796,10 @@
         <v>87</v>
       </c>
       <c r="D116" s="32" t="s">
+        <v>271</v>
+      </c>
+      <c r="E116" s="33" t="s">
         <v>272</v>
-      </c>
-      <c r="E116" s="33" t="s">
-        <v>273</v>
       </c>
       <c r="F116" s="34"/>
       <c r="G116" s="35"/>
@@ -7830,10 +7830,10 @@
         <v>87</v>
       </c>
       <c r="D117" s="32" t="s">
+        <v>273</v>
+      </c>
+      <c r="E117" s="33" t="s">
         <v>274</v>
-      </c>
-      <c r="E117" s="33" t="s">
-        <v>275</v>
       </c>
       <c r="F117" s="34"/>
       <c r="G117" s="35"/>
@@ -7864,10 +7864,10 @@
         <v>87</v>
       </c>
       <c r="D118" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="E118" s="33" t="s">
         <v>276</v>
-      </c>
-      <c r="E118" s="33" t="s">
-        <v>277</v>
       </c>
       <c r="F118" s="34"/>
       <c r="G118" s="35"/>
@@ -7898,10 +7898,10 @@
         <v>87</v>
       </c>
       <c r="D119" s="32" t="s">
+        <v>277</v>
+      </c>
+      <c r="E119" s="33" t="s">
         <v>278</v>
-      </c>
-      <c r="E119" s="33" t="s">
-        <v>279</v>
       </c>
       <c r="F119" s="34"/>
       <c r="G119" s="35"/>
@@ -7932,10 +7932,10 @@
         <v>87</v>
       </c>
       <c r="D120" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="E120" s="33" t="s">
         <v>280</v>
-      </c>
-      <c r="E120" s="33" t="s">
-        <v>281</v>
       </c>
       <c r="F120" s="34"/>
       <c r="G120" s="35"/>
@@ -7966,10 +7966,10 @@
         <v>87</v>
       </c>
       <c r="D121" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="E121" s="33" t="s">
         <v>282</v>
-      </c>
-      <c r="E121" s="33" t="s">
-        <v>283</v>
       </c>
       <c r="F121" s="34"/>
       <c r="G121" s="35"/>
@@ -8000,10 +8000,10 @@
         <v>87</v>
       </c>
       <c r="D122" s="32" t="s">
+        <v>283</v>
+      </c>
+      <c r="E122" s="33" t="s">
         <v>284</v>
-      </c>
-      <c r="E122" s="33" t="s">
-        <v>285</v>
       </c>
       <c r="F122" s="34"/>
       <c r="G122" s="35"/>
@@ -8034,10 +8034,10 @@
         <v>96</v>
       </c>
       <c r="D123" s="32" t="s">
+        <v>285</v>
+      </c>
+      <c r="E123" s="33" t="s">
         <v>286</v>
-      </c>
-      <c r="E123" s="33" t="s">
-        <v>287</v>
       </c>
       <c r="F123" s="34"/>
       <c r="G123" s="35"/>
@@ -8068,10 +8068,10 @@
         <v>96</v>
       </c>
       <c r="D124" s="32" t="s">
+        <v>287</v>
+      </c>
+      <c r="E124" s="33" t="s">
         <v>288</v>
-      </c>
-      <c r="E124" s="33" t="s">
-        <v>289</v>
       </c>
       <c r="F124" s="34"/>
       <c r="G124" s="35"/>
@@ -8102,10 +8102,10 @@
         <v>96</v>
       </c>
       <c r="D125" s="32" t="s">
+        <v>289</v>
+      </c>
+      <c r="E125" s="33" t="s">
         <v>290</v>
-      </c>
-      <c r="E125" s="33" t="s">
-        <v>291</v>
       </c>
       <c r="F125" s="34"/>
       <c r="G125" s="35"/>
@@ -8136,10 +8136,10 @@
         <v>96</v>
       </c>
       <c r="D126" s="32" t="s">
+        <v>291</v>
+      </c>
+      <c r="E126" s="33" t="s">
         <v>292</v>
-      </c>
-      <c r="E126" s="33" t="s">
-        <v>293</v>
       </c>
       <c r="F126" s="34"/>
       <c r="G126" s="35"/>
@@ -8170,10 +8170,10 @@
         <v>96</v>
       </c>
       <c r="D127" s="32" t="s">
+        <v>293</v>
+      </c>
+      <c r="E127" s="33" t="s">
         <v>294</v>
-      </c>
-      <c r="E127" s="33" t="s">
-        <v>295</v>
       </c>
       <c r="F127" s="34"/>
       <c r="G127" s="35"/>
@@ -8204,10 +8204,10 @@
         <v>96</v>
       </c>
       <c r="D128" s="32" t="s">
+        <v>295</v>
+      </c>
+      <c r="E128" s="33" t="s">
         <v>296</v>
-      </c>
-      <c r="E128" s="33" t="s">
-        <v>297</v>
       </c>
       <c r="F128" s="34"/>
       <c r="G128" s="35"/>
@@ -8238,10 +8238,10 @@
         <v>96</v>
       </c>
       <c r="D129" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="E129" s="33" t="s">
         <v>298</v>
-      </c>
-      <c r="E129" s="33" t="s">
-        <v>299</v>
       </c>
       <c r="F129" s="34"/>
       <c r="G129" s="35"/>
@@ -8272,10 +8272,10 @@
         <v>96</v>
       </c>
       <c r="D130" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="E130" s="33" t="s">
         <v>300</v>
-      </c>
-      <c r="E130" s="33" t="s">
-        <v>301</v>
       </c>
       <c r="F130" s="34"/>
       <c r="G130" s="35"/>
@@ -8306,10 +8306,10 @@
         <v>96</v>
       </c>
       <c r="D131" s="32" t="s">
+        <v>301</v>
+      </c>
+      <c r="E131" s="33" t="s">
         <v>302</v>
-      </c>
-      <c r="E131" s="33" t="s">
-        <v>303</v>
       </c>
       <c r="F131" s="34"/>
       <c r="G131" s="35"/>
@@ -8340,10 +8340,10 @@
         <v>96</v>
       </c>
       <c r="D132" s="32" t="s">
+        <v>303</v>
+      </c>
+      <c r="E132" s="33" t="s">
         <v>304</v>
-      </c>
-      <c r="E132" s="33" t="s">
-        <v>305</v>
       </c>
       <c r="F132" s="34"/>
       <c r="G132" s="35"/>
@@ -8374,10 +8374,10 @@
         <v>96</v>
       </c>
       <c r="D133" s="32" t="s">
+        <v>305</v>
+      </c>
+      <c r="E133" s="33" t="s">
         <v>306</v>
-      </c>
-      <c r="E133" s="33" t="s">
-        <v>307</v>
       </c>
       <c r="F133" s="34"/>
       <c r="G133" s="35"/>
@@ -8408,10 +8408,10 @@
         <v>96</v>
       </c>
       <c r="D134" s="32" t="s">
+        <v>307</v>
+      </c>
+      <c r="E134" s="33" t="s">
         <v>308</v>
-      </c>
-      <c r="E134" s="33" t="s">
-        <v>309</v>
       </c>
       <c r="F134" s="34"/>
       <c r="G134" s="35"/>
@@ -8442,10 +8442,10 @@
         <v>96</v>
       </c>
       <c r="D135" s="32" t="s">
+        <v>309</v>
+      </c>
+      <c r="E135" s="33" t="s">
         <v>310</v>
-      </c>
-      <c r="E135" s="33" t="s">
-        <v>311</v>
       </c>
       <c r="F135" s="34"/>
       <c r="G135" s="35"/>
@@ -8476,10 +8476,10 @@
         <v>96</v>
       </c>
       <c r="D136" s="32" t="s">
+        <v>311</v>
+      </c>
+      <c r="E136" s="33" t="s">
         <v>312</v>
-      </c>
-      <c r="E136" s="33" t="s">
-        <v>313</v>
       </c>
       <c r="F136" s="34"/>
       <c r="G136" s="35"/>
@@ -8510,10 +8510,10 @@
         <v>96</v>
       </c>
       <c r="D137" s="32" t="s">
+        <v>313</v>
+      </c>
+      <c r="E137" s="33" t="s">
         <v>314</v>
-      </c>
-      <c r="E137" s="33" t="s">
-        <v>315</v>
       </c>
       <c r="F137" s="34"/>
       <c r="G137" s="35"/>
@@ -8544,10 +8544,10 @@
         <v>96</v>
       </c>
       <c r="D138" s="32" t="s">
+        <v>315</v>
+      </c>
+      <c r="E138" s="33" t="s">
         <v>316</v>
-      </c>
-      <c r="E138" s="33" t="s">
-        <v>317</v>
       </c>
       <c r="F138" s="34"/>
       <c r="G138" s="35"/>
@@ -8578,10 +8578,10 @@
         <v>96</v>
       </c>
       <c r="D139" s="32" t="s">
+        <v>317</v>
+      </c>
+      <c r="E139" s="33" t="s">
         <v>318</v>
-      </c>
-      <c r="E139" s="33" t="s">
-        <v>319</v>
       </c>
       <c r="F139" s="34"/>
       <c r="G139" s="35"/>
@@ -8612,10 +8612,10 @@
         <v>96</v>
       </c>
       <c r="D140" s="32" t="s">
+        <v>319</v>
+      </c>
+      <c r="E140" s="33" t="s">
         <v>320</v>
-      </c>
-      <c r="E140" s="33" t="s">
-        <v>321</v>
       </c>
       <c r="F140" s="34"/>
       <c r="G140" s="35"/>
@@ -8646,10 +8646,10 @@
         <v>96</v>
       </c>
       <c r="D141" s="32" t="s">
+        <v>321</v>
+      </c>
+      <c r="E141" s="33" t="s">
         <v>322</v>
-      </c>
-      <c r="E141" s="33" t="s">
-        <v>323</v>
       </c>
       <c r="F141" s="34"/>
       <c r="G141" s="35"/>
@@ -8680,10 +8680,10 @@
         <v>96</v>
       </c>
       <c r="D142" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="E142" s="33" t="s">
         <v>324</v>
-      </c>
-      <c r="E142" s="33" t="s">
-        <v>325</v>
       </c>
       <c r="F142" s="34"/>
       <c r="G142" s="35"/>
@@ -8714,10 +8714,10 @@
         <v>96</v>
       </c>
       <c r="D143" s="32" t="s">
+        <v>325</v>
+      </c>
+      <c r="E143" s="33" t="s">
         <v>326</v>
-      </c>
-      <c r="E143" s="33" t="s">
-        <v>327</v>
       </c>
       <c r="F143" s="34"/>
       <c r="G143" s="35"/>
@@ -8748,10 +8748,10 @@
         <v>96</v>
       </c>
       <c r="D144" s="32" t="s">
+        <v>327</v>
+      </c>
+      <c r="E144" s="33" t="s">
         <v>328</v>
-      </c>
-      <c r="E144" s="33" t="s">
-        <v>329</v>
       </c>
       <c r="F144" s="34"/>
       <c r="G144" s="35"/>
@@ -8782,10 +8782,10 @@
         <v>96</v>
       </c>
       <c r="D145" s="32" t="s">
+        <v>329</v>
+      </c>
+      <c r="E145" s="33" t="s">
         <v>330</v>
-      </c>
-      <c r="E145" s="33" t="s">
-        <v>331</v>
       </c>
       <c r="F145" s="34"/>
       <c r="G145" s="35"/>
@@ -8816,10 +8816,10 @@
         <v>96</v>
       </c>
       <c r="D146" s="32" t="s">
+        <v>331</v>
+      </c>
+      <c r="E146" s="33" t="s">
         <v>332</v>
-      </c>
-      <c r="E146" s="33" t="s">
-        <v>333</v>
       </c>
       <c r="F146" s="34"/>
       <c r="G146" s="35"/>
@@ -8850,10 +8850,10 @@
         <v>96</v>
       </c>
       <c r="D147" s="32" t="s">
+        <v>333</v>
+      </c>
+      <c r="E147" s="33" t="s">
         <v>334</v>
-      </c>
-      <c r="E147" s="33" t="s">
-        <v>335</v>
       </c>
       <c r="F147" s="34"/>
       <c r="G147" s="35"/>
@@ -23243,6 +23243,11 @@
     <filterColumn colId="2">
       <filters>
         <filter val="RAD"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="9">
+      <filters>
+        <filter val="NO"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -23311,10 +23316,10 @@
         <v>25</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>336</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -23322,13 +23327,13 @@
         <v>45</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>338</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="13" t="s">
         <v>339</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -23336,13 +23341,13 @@
         <v>57</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C3" s="16" t="s">
+        <v>340</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>341</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -23350,13 +23355,13 @@
         <v>66</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C4" s="16" t="s">
+        <v>342</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>343</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -23364,13 +23369,13 @@
         <v>78</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C5" s="16" t="s">
+        <v>344</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>345</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -23378,13 +23383,13 @@
         <v>87</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C6" s="16" t="s">
+        <v>346</v>
+      </c>
+      <c r="D6" s="17" t="s">
         <v>347</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -23392,13 +23397,13 @@
         <v>96</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C7" s="20" t="s">
+        <v>348</v>
+      </c>
+      <c r="D7" s="17" t="s">
         <v>349</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -24421,7 +24426,7 @@
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B2" s="45" t="s">
         <v>69</v>
@@ -24429,7 +24434,7 @@
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B3" s="45" t="s">
         <v>74</v>

</xml_diff>